<commit_message>
Version 2 pcb complete
</commit_message>
<xml_diff>
--- a/Documentation/BOM_Truss_PCB.xlsx
+++ b/Documentation/BOM_Truss_PCB.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="BOM_Truss_PCB" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterate="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -935,9 +935,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -955,6 +952,9 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1282,14 +1282,14 @@
   </sheetPr>
   <dimension ref="A1:I214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20" style="11" customWidth="1"/>
+    <col min="2" max="2" width="20" style="10" customWidth="1"/>
     <col min="3" max="3" width="20.28515625" customWidth="1"/>
     <col min="4" max="4" width="20.5703125" customWidth="1"/>
     <col min="5" max="5" width="39" style="3" customWidth="1"/>
@@ -1300,13 +1300,13 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
@@ -1315,12 +1315,12 @@
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="8">
         <v>44749.631249999999</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
-      <c r="E2" s="13"/>
+      <c r="E2" s="12"/>
       <c r="F2" s="7"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -1335,7 +1335,7 @@
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
-      <c r="E3" s="13"/>
+      <c r="E3" s="12"/>
       <c r="F3" s="7"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -1345,13 +1345,13 @@
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -1365,7 +1365,7 @@
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="13"/>
+      <c r="E5" s="12"/>
       <c r="F5" s="7"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -1375,7 +1375,7 @@
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -1384,7 +1384,7 @@
       <c r="D6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="13" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="5" t="s">
@@ -1401,7 +1401,7 @@
       <c r="B7" s="6"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="12"/>
+      <c r="E7" s="11"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -1420,7 +1420,7 @@
       <c r="D8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="11" t="s">
         <v>17</v>
       </c>
       <c r="F8" s="4" t="s">
@@ -1435,7 +1435,7 @@
       <c r="B9" s="6"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="12"/>
+      <c r="E9" s="11"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
@@ -1454,7 +1454,7 @@
       <c r="D10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="11" t="s">
         <v>22</v>
       </c>
       <c r="F10" s="4" t="s">
@@ -1477,7 +1477,7 @@
       <c r="D11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="11" t="s">
         <v>27</v>
       </c>
       <c r="F11" s="4" t="s">
@@ -1500,7 +1500,7 @@
       <c r="D12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="11" t="s">
         <v>22</v>
       </c>
       <c r="F12" s="4" t="s">
@@ -1515,7 +1515,7 @@
       <c r="B13" s="6"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="12"/>
+      <c r="E13" s="11"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
@@ -1534,7 +1534,7 @@
       <c r="D14" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="11" t="s">
         <v>33</v>
       </c>
       <c r="F14" s="4" t="s">
@@ -1557,7 +1557,7 @@
       <c r="D15" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="11" t="s">
         <v>37</v>
       </c>
       <c r="F15" s="4" t="s">
@@ -1580,7 +1580,7 @@
       <c r="D16" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="11" t="s">
         <v>33</v>
       </c>
       <c r="F16" s="4" t="s">
@@ -1603,7 +1603,7 @@
       <c r="D17" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="11" t="s">
         <v>42</v>
       </c>
       <c r="F17" s="4" t="s">
@@ -1626,7 +1626,7 @@
       <c r="D18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="11" t="s">
         <v>33</v>
       </c>
       <c r="F18" s="4" t="s">
@@ -1649,7 +1649,7 @@
       <c r="D19" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="11" t="s">
         <v>33</v>
       </c>
       <c r="F19" s="4" t="s">
@@ -1672,7 +1672,7 @@
       <c r="D20" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="11" t="s">
         <v>33</v>
       </c>
       <c r="F20" s="4" t="s">
@@ -1695,7 +1695,7 @@
       <c r="D21" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E21" s="11" t="s">
         <v>33</v>
       </c>
       <c r="F21" s="4" t="s">
@@ -1710,7 +1710,7 @@
       <c r="B22" s="6"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="12"/>
+      <c r="E22" s="11"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
@@ -1729,7 +1729,7 @@
       <c r="D23" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E23" s="11" t="s">
         <v>51</v>
       </c>
       <c r="F23" s="4" t="s">
@@ -1752,7 +1752,7 @@
       <c r="D24" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E24" s="11" t="s">
         <v>27</v>
       </c>
       <c r="F24" s="4" t="s">
@@ -1775,7 +1775,7 @@
       <c r="D25" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="E25" s="11" t="s">
         <v>51</v>
       </c>
       <c r="F25" s="4" t="s">
@@ -1790,7 +1790,7 @@
       <c r="B26" s="6"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
-      <c r="E26" s="12"/>
+      <c r="E26" s="11"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
@@ -1809,7 +1809,7 @@
       <c r="D27" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="E27" s="11" t="s">
         <v>57</v>
       </c>
       <c r="F27" s="4" t="s">
@@ -1824,7 +1824,7 @@
       <c r="B28" s="6"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
-      <c r="E28" s="12"/>
+      <c r="E28" s="11"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
@@ -1843,7 +1843,7 @@
       <c r="D29" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="E29" s="11" t="s">
         <v>60</v>
       </c>
       <c r="F29" s="4" t="s">
@@ -1858,7 +1858,7 @@
       <c r="B30" s="6"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
-      <c r="E30" s="12"/>
+      <c r="E30" s="11"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
@@ -1877,10 +1877,10 @@
       <c r="D31" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="E31" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="F31" s="12" t="s">
+      <c r="F31" s="11" t="s">
         <v>65</v>
       </c>
       <c r="G31" s="4"/>
@@ -1900,10 +1900,10 @@
       <c r="D32" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E32" s="12" t="s">
+      <c r="E32" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="12" t="s">
+      <c r="F32" s="11" t="s">
         <v>65</v>
       </c>
       <c r="G32" s="4"/>
@@ -1923,10 +1923,10 @@
       <c r="D33" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E33" s="12" t="s">
+      <c r="E33" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="F33" s="12" t="s">
+      <c r="F33" s="11" t="s">
         <v>74</v>
       </c>
       <c r="G33" s="4"/>
@@ -1946,10 +1946,10 @@
       <c r="D34" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E34" s="12" t="s">
+      <c r="E34" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="F34" s="12" t="s">
+      <c r="F34" s="11" t="s">
         <v>79</v>
       </c>
       <c r="G34" s="4"/>
@@ -1961,7 +1961,7 @@
       <c r="B35" s="6"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
-      <c r="E35" s="12"/>
+      <c r="E35" s="11"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
@@ -1980,7 +1980,7 @@
       <c r="D36" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E36" s="12" t="s">
+      <c r="E36" s="11" t="s">
         <v>83</v>
       </c>
       <c r="F36" s="4" t="s">
@@ -1995,7 +1995,7 @@
       <c r="B37" s="6"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
-      <c r="E37" s="12"/>
+      <c r="E37" s="11"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
@@ -2014,10 +2014,10 @@
       <c r="D38" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E38" s="12" t="s">
+      <c r="E38" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="F38" s="12" t="s">
+      <c r="F38" s="11" t="s">
         <v>88</v>
       </c>
       <c r="G38" s="4"/>
@@ -2037,10 +2037,10 @@
       <c r="D39" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E39" s="12" t="s">
+      <c r="E39" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="F39" s="12" t="s">
+      <c r="F39" s="11" t="s">
         <v>92</v>
       </c>
       <c r="G39" s="4"/>
@@ -2052,8 +2052,8 @@
       <c r="B40" s="6"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
@@ -2071,10 +2071,10 @@
       <c r="D41" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E41" s="12" t="s">
+      <c r="E41" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="F41" s="12" t="s">
+      <c r="F41" s="11" t="s">
         <v>97</v>
       </c>
       <c r="G41" s="4"/>
@@ -2094,10 +2094,10 @@
       <c r="D42" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E42" s="12" t="s">
+      <c r="E42" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="F42" s="12" t="s">
+      <c r="F42" s="11" t="s">
         <v>97</v>
       </c>
       <c r="G42" s="4"/>
@@ -2117,10 +2117,10 @@
       <c r="D43" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E43" s="12" t="s">
+      <c r="E43" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="F43" s="12" t="s">
+      <c r="F43" s="11" t="s">
         <v>97</v>
       </c>
       <c r="G43" s="4"/>
@@ -2140,10 +2140,10 @@
       <c r="D44" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E44" s="12" t="s">
+      <c r="E44" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="F44" s="12" t="s">
+      <c r="F44" s="11" t="s">
         <v>97</v>
       </c>
       <c r="G44" s="4"/>
@@ -2163,10 +2163,10 @@
       <c r="D45" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E45" s="12" t="s">
+      <c r="E45" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="F45" s="12" t="s">
+      <c r="F45" s="11" t="s">
         <v>97</v>
       </c>
       <c r="G45" s="4"/>
@@ -2186,10 +2186,10 @@
       <c r="D46" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E46" s="12" t="s">
+      <c r="E46" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="F46" s="12" t="s">
+      <c r="F46" s="11" t="s">
         <v>97</v>
       </c>
       <c r="G46" s="4"/>
@@ -2209,10 +2209,10 @@
       <c r="D47" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E47" s="12" t="s">
+      <c r="E47" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="F47" s="12" t="s">
+      <c r="F47" s="11" t="s">
         <v>97</v>
       </c>
       <c r="G47" s="4"/>
@@ -2232,10 +2232,10 @@
       <c r="D48" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E48" s="12" t="s">
+      <c r="E48" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="F48" s="12" t="s">
+      <c r="F48" s="11" t="s">
         <v>97</v>
       </c>
       <c r="G48" s="4"/>
@@ -2255,10 +2255,10 @@
       <c r="D49" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E49" s="12" t="s">
+      <c r="E49" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="F49" s="12" t="s">
+      <c r="F49" s="11" t="s">
         <v>97</v>
       </c>
       <c r="G49" s="4"/>
@@ -2270,8 +2270,8 @@
       <c r="B50" s="6"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="12"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
@@ -2289,10 +2289,10 @@
       <c r="D51" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="E51" s="12" t="s">
+      <c r="E51" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="F51" s="12" t="s">
+      <c r="F51" s="11" t="s">
         <v>118</v>
       </c>
       <c r="G51" s="4"/>
@@ -2312,10 +2312,10 @@
       <c r="D52" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="E52" s="12" t="s">
+      <c r="E52" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="F52" s="12" t="s">
+      <c r="F52" s="11" t="s">
         <v>122</v>
       </c>
       <c r="G52" s="4"/>
@@ -2335,10 +2335,10 @@
       <c r="D53" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="E53" s="12" t="s">
+      <c r="E53" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="F53" s="12" t="s">
+      <c r="F53" s="11" t="s">
         <v>126</v>
       </c>
       <c r="G53" s="4"/>
@@ -2358,10 +2358,10 @@
       <c r="D54" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="E54" s="12" t="s">
+      <c r="E54" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="F54" s="12" t="s">
+      <c r="F54" s="11" t="s">
         <v>129</v>
       </c>
       <c r="G54" s="4"/>
@@ -2373,8 +2373,8 @@
       <c r="B55" s="6"/>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="11"/>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
@@ -2384,8 +2384,8 @@
       <c r="B56" s="6"/>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
-      <c r="E56" s="12"/>
-      <c r="F56" s="12"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
@@ -2395,8 +2395,8 @@
       <c r="B57" s="6"/>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
-      <c r="E57" s="12"/>
-      <c r="F57" s="12"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
       <c r="G57" s="4"/>
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
@@ -2406,8 +2406,8 @@
       <c r="B58" s="6"/>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
-      <c r="E58" s="12"/>
-      <c r="F58" s="12"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="11"/>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
@@ -2417,8 +2417,8 @@
       <c r="B59" s="6"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
-      <c r="E59" s="12"/>
-      <c r="F59" s="12"/>
+      <c r="E59" s="11"/>
+      <c r="F59" s="11"/>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
@@ -2428,8 +2428,8 @@
       <c r="B60" s="6"/>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
-      <c r="E60" s="12"/>
-      <c r="F60" s="12"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
@@ -2439,8 +2439,8 @@
       <c r="B61" s="6"/>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
-      <c r="E61" s="12"/>
-      <c r="F61" s="12"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
@@ -2450,8 +2450,8 @@
       <c r="B62" s="6"/>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
-      <c r="E62" s="12"/>
-      <c r="F62" s="12"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="11"/>
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
       <c r="I62" s="4"/>
@@ -2461,8 +2461,8 @@
       <c r="B63" s="6"/>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
-      <c r="E63" s="12"/>
-      <c r="F63" s="12"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
       <c r="G63" s="4"/>
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
@@ -2472,8 +2472,8 @@
       <c r="B64" s="6"/>
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
-      <c r="E64" s="12"/>
-      <c r="F64" s="12"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
       <c r="G64" s="4"/>
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
@@ -2483,8 +2483,8 @@
       <c r="B65" s="6"/>
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
-      <c r="E65" s="12"/>
-      <c r="F65" s="12"/>
+      <c r="E65" s="11"/>
+      <c r="F65" s="11"/>
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
       <c r="I65" s="4"/>
@@ -2494,8 +2494,8 @@
       <c r="B66" s="6"/>
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
-      <c r="E66" s="12"/>
-      <c r="F66" s="12"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
       <c r="G66" s="4"/>
       <c r="H66" s="4"/>
       <c r="I66" s="4"/>
@@ -2505,8 +2505,8 @@
       <c r="B67" s="6"/>
       <c r="C67" s="4"/>
       <c r="D67" s="4"/>
-      <c r="E67" s="12"/>
-      <c r="F67" s="12"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
       <c r="G67" s="4"/>
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
@@ -2516,8 +2516,8 @@
       <c r="B68" s="6"/>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
-      <c r="E68" s="12"/>
-      <c r="F68" s="12"/>
+      <c r="E68" s="11"/>
+      <c r="F68" s="11"/>
       <c r="G68" s="4"/>
       <c r="H68" s="4"/>
       <c r="I68" s="4"/>
@@ -2527,8 +2527,8 @@
       <c r="B69" s="6"/>
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
-      <c r="E69" s="12"/>
-      <c r="F69" s="12"/>
+      <c r="E69" s="11"/>
+      <c r="F69" s="11"/>
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
       <c r="I69" s="4"/>
@@ -2538,8 +2538,8 @@
       <c r="B70" s="6"/>
       <c r="C70" s="4"/>
       <c r="D70" s="4"/>
-      <c r="E70" s="12"/>
-      <c r="F70" s="12"/>
+      <c r="E70" s="11"/>
+      <c r="F70" s="11"/>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
@@ -2549,8 +2549,8 @@
       <c r="B71" s="6"/>
       <c r="C71" s="4"/>
       <c r="D71" s="4"/>
-      <c r="E71" s="12"/>
-      <c r="F71" s="12"/>
+      <c r="E71" s="11"/>
+      <c r="F71" s="11"/>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
       <c r="I71" s="4"/>
@@ -2560,8 +2560,8 @@
       <c r="B72" s="6"/>
       <c r="C72" s="4"/>
       <c r="D72" s="4"/>
-      <c r="E72" s="12"/>
-      <c r="F72" s="12"/>
+      <c r="E72" s="11"/>
+      <c r="F72" s="11"/>
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
@@ -2571,8 +2571,8 @@
       <c r="B73" s="6"/>
       <c r="C73" s="4"/>
       <c r="D73" s="4"/>
-      <c r="E73" s="12"/>
-      <c r="F73" s="12"/>
+      <c r="E73" s="11"/>
+      <c r="F73" s="11"/>
       <c r="G73" s="4"/>
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
@@ -2582,8 +2582,8 @@
       <c r="B74" s="6"/>
       <c r="C74" s="4"/>
       <c r="D74" s="4"/>
-      <c r="E74" s="12"/>
-      <c r="F74" s="12"/>
+      <c r="E74" s="11"/>
+      <c r="F74" s="11"/>
       <c r="G74" s="4"/>
       <c r="H74" s="4"/>
       <c r="I74" s="4"/>
@@ -2593,8 +2593,8 @@
       <c r="B75" s="6"/>
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
-      <c r="E75" s="12"/>
-      <c r="F75" s="12"/>
+      <c r="E75" s="11"/>
+      <c r="F75" s="11"/>
       <c r="G75" s="4"/>
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
@@ -2604,8 +2604,8 @@
       <c r="B76" s="6"/>
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
-      <c r="E76" s="12"/>
-      <c r="F76" s="12"/>
+      <c r="E76" s="11"/>
+      <c r="F76" s="11"/>
       <c r="G76" s="4"/>
       <c r="H76" s="4"/>
       <c r="I76" s="4"/>
@@ -2615,8 +2615,8 @@
       <c r="B77" s="6"/>
       <c r="C77" s="4"/>
       <c r="D77" s="4"/>
-      <c r="E77" s="12"/>
-      <c r="F77" s="12"/>
+      <c r="E77" s="11"/>
+      <c r="F77" s="11"/>
       <c r="G77" s="4"/>
       <c r="H77" s="4"/>
       <c r="I77" s="4"/>
@@ -2626,8 +2626,8 @@
       <c r="B78" s="6"/>
       <c r="C78" s="4"/>
       <c r="D78" s="4"/>
-      <c r="E78" s="12"/>
-      <c r="F78" s="12"/>
+      <c r="E78" s="11"/>
+      <c r="F78" s="11"/>
       <c r="G78" s="4"/>
       <c r="H78" s="4"/>
       <c r="I78" s="4"/>
@@ -2637,8 +2637,8 @@
       <c r="B79" s="6"/>
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
-      <c r="E79" s="12"/>
-      <c r="F79" s="12"/>
+      <c r="E79" s="11"/>
+      <c r="F79" s="11"/>
       <c r="G79" s="4"/>
       <c r="H79" s="4"/>
       <c r="I79" s="4"/>
@@ -2648,8 +2648,8 @@
       <c r="B80" s="6"/>
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
-      <c r="E80" s="12"/>
-      <c r="F80" s="12"/>
+      <c r="E80" s="11"/>
+      <c r="F80" s="11"/>
       <c r="G80" s="4"/>
       <c r="H80" s="4"/>
       <c r="I80" s="4"/>
@@ -2659,8 +2659,8 @@
       <c r="B81" s="6"/>
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
-      <c r="E81" s="12"/>
-      <c r="F81" s="12"/>
+      <c r="E81" s="11"/>
+      <c r="F81" s="11"/>
       <c r="G81" s="4"/>
       <c r="H81" s="4"/>
       <c r="I81" s="4"/>
@@ -2670,8 +2670,8 @@
       <c r="B82" s="6"/>
       <c r="C82" s="4"/>
       <c r="D82" s="4"/>
-      <c r="E82" s="12"/>
-      <c r="F82" s="12"/>
+      <c r="E82" s="11"/>
+      <c r="F82" s="11"/>
       <c r="G82" s="4"/>
       <c r="H82" s="4"/>
       <c r="I82" s="4"/>
@@ -2681,8 +2681,8 @@
       <c r="B83" s="6"/>
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
-      <c r="E83" s="12"/>
-      <c r="F83" s="12"/>
+      <c r="E83" s="11"/>
+      <c r="F83" s="11"/>
       <c r="G83" s="4"/>
       <c r="H83" s="4"/>
       <c r="I83" s="4"/>
@@ -2692,8 +2692,8 @@
       <c r="B84" s="6"/>
       <c r="C84" s="4"/>
       <c r="D84" s="4"/>
-      <c r="E84" s="12"/>
-      <c r="F84" s="12"/>
+      <c r="E84" s="11"/>
+      <c r="F84" s="11"/>
       <c r="G84" s="4"/>
       <c r="H84" s="4"/>
       <c r="I84" s="4"/>
@@ -2703,8 +2703,8 @@
       <c r="B85" s="6"/>
       <c r="C85" s="4"/>
       <c r="D85" s="4"/>
-      <c r="E85" s="12"/>
-      <c r="F85" s="12"/>
+      <c r="E85" s="11"/>
+      <c r="F85" s="11"/>
       <c r="G85" s="4"/>
       <c r="H85" s="4"/>
       <c r="I85" s="4"/>
@@ -2714,8 +2714,8 @@
       <c r="B86" s="6"/>
       <c r="C86" s="4"/>
       <c r="D86" s="4"/>
-      <c r="E86" s="12"/>
-      <c r="F86" s="12"/>
+      <c r="E86" s="11"/>
+      <c r="F86" s="11"/>
       <c r="G86" s="4"/>
       <c r="H86" s="4"/>
       <c r="I86" s="4"/>
@@ -2725,8 +2725,8 @@
       <c r="B87" s="6"/>
       <c r="C87" s="4"/>
       <c r="D87" s="4"/>
-      <c r="E87" s="12"/>
-      <c r="F87" s="12"/>
+      <c r="E87" s="11"/>
+      <c r="F87" s="11"/>
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
       <c r="I87" s="4"/>
@@ -2736,8 +2736,8 @@
       <c r="B88" s="6"/>
       <c r="C88" s="4"/>
       <c r="D88" s="4"/>
-      <c r="E88" s="12"/>
-      <c r="F88" s="12"/>
+      <c r="E88" s="11"/>
+      <c r="F88" s="11"/>
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
       <c r="I88" s="4"/>
@@ -2747,8 +2747,8 @@
       <c r="B89" s="6"/>
       <c r="C89" s="4"/>
       <c r="D89" s="4"/>
-      <c r="E89" s="12"/>
-      <c r="F89" s="12"/>
+      <c r="E89" s="11"/>
+      <c r="F89" s="11"/>
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
       <c r="I89" s="4"/>
@@ -2758,8 +2758,8 @@
       <c r="B90" s="6"/>
       <c r="C90" s="4"/>
       <c r="D90" s="4"/>
-      <c r="E90" s="12"/>
-      <c r="F90" s="12"/>
+      <c r="E90" s="11"/>
+      <c r="F90" s="11"/>
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
       <c r="I90" s="4"/>
@@ -2769,8 +2769,8 @@
       <c r="B91" s="6"/>
       <c r="C91" s="4"/>
       <c r="D91" s="4"/>
-      <c r="E91" s="12"/>
-      <c r="F91" s="12"/>
+      <c r="E91" s="11"/>
+      <c r="F91" s="11"/>
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
       <c r="I91" s="4"/>
@@ -2780,8 +2780,8 @@
       <c r="B92" s="6"/>
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
-      <c r="E92" s="12"/>
-      <c r="F92" s="12"/>
+      <c r="E92" s="11"/>
+      <c r="F92" s="11"/>
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
       <c r="I92" s="4"/>
@@ -2791,8 +2791,8 @@
       <c r="B93" s="6"/>
       <c r="C93" s="4"/>
       <c r="D93" s="4"/>
-      <c r="E93" s="12"/>
-      <c r="F93" s="12"/>
+      <c r="E93" s="11"/>
+      <c r="F93" s="11"/>
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
       <c r="I93" s="4"/>
@@ -2802,8 +2802,8 @@
       <c r="B94" s="6"/>
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
-      <c r="E94" s="12"/>
-      <c r="F94" s="12"/>
+      <c r="E94" s="11"/>
+      <c r="F94" s="11"/>
       <c r="G94" s="4"/>
       <c r="H94" s="4"/>
       <c r="I94" s="4"/>
@@ -2813,8 +2813,8 @@
       <c r="B95" s="6"/>
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
-      <c r="E95" s="12"/>
-      <c r="F95" s="12"/>
+      <c r="E95" s="11"/>
+      <c r="F95" s="11"/>
       <c r="G95" s="4"/>
       <c r="H95" s="4"/>
       <c r="I95" s="4"/>
@@ -2824,8 +2824,8 @@
       <c r="B96" s="6"/>
       <c r="C96" s="4"/>
       <c r="D96" s="4"/>
-      <c r="E96" s="12"/>
-      <c r="F96" s="12"/>
+      <c r="E96" s="11"/>
+      <c r="F96" s="11"/>
       <c r="G96" s="4"/>
       <c r="H96" s="4"/>
       <c r="I96" s="4"/>
@@ -2835,8 +2835,8 @@
       <c r="B97" s="6"/>
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
-      <c r="E97" s="12"/>
-      <c r="F97" s="12"/>
+      <c r="E97" s="11"/>
+      <c r="F97" s="11"/>
       <c r="G97" s="4"/>
       <c r="H97" s="4"/>
       <c r="I97" s="4"/>
@@ -2846,8 +2846,8 @@
       <c r="B98" s="6"/>
       <c r="C98" s="4"/>
       <c r="D98" s="4"/>
-      <c r="E98" s="12"/>
-      <c r="F98" s="12"/>
+      <c r="E98" s="11"/>
+      <c r="F98" s="11"/>
       <c r="G98" s="4"/>
       <c r="H98" s="4"/>
       <c r="I98" s="4"/>
@@ -2857,8 +2857,8 @@
       <c r="B99" s="6"/>
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
-      <c r="E99" s="12"/>
-      <c r="F99" s="12"/>
+      <c r="E99" s="11"/>
+      <c r="F99" s="11"/>
       <c r="G99" s="4"/>
       <c r="H99" s="4"/>
       <c r="I99" s="4"/>
@@ -2868,8 +2868,8 @@
       <c r="B100" s="6"/>
       <c r="C100" s="4"/>
       <c r="D100" s="4"/>
-      <c r="E100" s="12"/>
-      <c r="F100" s="12"/>
+      <c r="E100" s="11"/>
+      <c r="F100" s="11"/>
       <c r="G100" s="4"/>
       <c r="H100" s="4"/>
       <c r="I100" s="4"/>
@@ -2879,8 +2879,8 @@
       <c r="B101" s="6"/>
       <c r="C101" s="4"/>
       <c r="D101" s="4"/>
-      <c r="E101" s="12"/>
-      <c r="F101" s="12"/>
+      <c r="E101" s="11"/>
+      <c r="F101" s="11"/>
       <c r="G101" s="4"/>
       <c r="H101" s="4"/>
       <c r="I101" s="4"/>
@@ -2890,8 +2890,8 @@
       <c r="B102" s="6"/>
       <c r="C102" s="4"/>
       <c r="D102" s="4"/>
-      <c r="E102" s="12"/>
-      <c r="F102" s="12"/>
+      <c r="E102" s="11"/>
+      <c r="F102" s="11"/>
       <c r="G102" s="4"/>
       <c r="H102" s="4"/>
       <c r="I102" s="4"/>
@@ -2901,8 +2901,8 @@
       <c r="B103" s="6"/>
       <c r="C103" s="4"/>
       <c r="D103" s="4"/>
-      <c r="E103" s="12"/>
-      <c r="F103" s="12"/>
+      <c r="E103" s="11"/>
+      <c r="F103" s="11"/>
       <c r="G103" s="4"/>
       <c r="H103" s="4"/>
       <c r="I103" s="4"/>
@@ -2912,8 +2912,8 @@
       <c r="B104" s="6"/>
       <c r="C104" s="4"/>
       <c r="D104" s="4"/>
-      <c r="E104" s="12"/>
-      <c r="F104" s="12"/>
+      <c r="E104" s="11"/>
+      <c r="F104" s="11"/>
       <c r="G104" s="4"/>
       <c r="H104" s="4"/>
       <c r="I104" s="4"/>
@@ -2923,8 +2923,8 @@
       <c r="B105" s="6"/>
       <c r="C105" s="4"/>
       <c r="D105" s="4"/>
-      <c r="E105" s="12"/>
-      <c r="F105" s="12"/>
+      <c r="E105" s="11"/>
+      <c r="F105" s="11"/>
       <c r="G105" s="4"/>
       <c r="H105" s="4"/>
       <c r="I105" s="4"/>
@@ -2934,8 +2934,8 @@
       <c r="B106" s="6"/>
       <c r="C106" s="4"/>
       <c r="D106" s="4"/>
-      <c r="E106" s="12"/>
-      <c r="F106" s="12"/>
+      <c r="E106" s="11"/>
+      <c r="F106" s="11"/>
       <c r="G106" s="4"/>
       <c r="H106" s="4"/>
       <c r="I106" s="4"/>
@@ -2945,8 +2945,8 @@
       <c r="B107" s="6"/>
       <c r="C107" s="4"/>
       <c r="D107" s="4"/>
-      <c r="E107" s="12"/>
-      <c r="F107" s="12"/>
+      <c r="E107" s="11"/>
+      <c r="F107" s="11"/>
       <c r="G107" s="4"/>
       <c r="H107" s="4"/>
       <c r="I107" s="4"/>
@@ -2956,8 +2956,8 @@
       <c r="B108" s="6"/>
       <c r="C108" s="4"/>
       <c r="D108" s="4"/>
-      <c r="E108" s="12"/>
-      <c r="F108" s="12"/>
+      <c r="E108" s="11"/>
+      <c r="F108" s="11"/>
       <c r="G108" s="4"/>
       <c r="H108" s="4"/>
       <c r="I108" s="4"/>
@@ -2967,8 +2967,8 @@
       <c r="B109" s="6"/>
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
-      <c r="E109" s="12"/>
-      <c r="F109" s="12"/>
+      <c r="E109" s="11"/>
+      <c r="F109" s="11"/>
       <c r="G109" s="4"/>
       <c r="H109" s="4"/>
       <c r="I109" s="4"/>
@@ -2978,8 +2978,8 @@
       <c r="B110" s="6"/>
       <c r="C110" s="4"/>
       <c r="D110" s="4"/>
-      <c r="E110" s="12"/>
-      <c r="F110" s="12"/>
+      <c r="E110" s="11"/>
+      <c r="F110" s="11"/>
       <c r="G110" s="4"/>
       <c r="H110" s="4"/>
       <c r="I110" s="4"/>
@@ -2989,8 +2989,8 @@
       <c r="B111" s="6"/>
       <c r="C111" s="4"/>
       <c r="D111" s="4"/>
-      <c r="E111" s="12"/>
-      <c r="F111" s="12"/>
+      <c r="E111" s="11"/>
+      <c r="F111" s="11"/>
       <c r="G111" s="4"/>
       <c r="H111" s="4"/>
       <c r="I111" s="4"/>
@@ -3000,8 +3000,8 @@
       <c r="B112" s="6"/>
       <c r="C112" s="4"/>
       <c r="D112" s="4"/>
-      <c r="E112" s="12"/>
-      <c r="F112" s="12"/>
+      <c r="E112" s="11"/>
+      <c r="F112" s="11"/>
       <c r="G112" s="4"/>
       <c r="H112" s="4"/>
       <c r="I112" s="4"/>
@@ -3011,8 +3011,8 @@
       <c r="B113" s="6"/>
       <c r="C113" s="4"/>
       <c r="D113" s="4"/>
-      <c r="E113" s="12"/>
-      <c r="F113" s="12"/>
+      <c r="E113" s="11"/>
+      <c r="F113" s="11"/>
       <c r="G113" s="4"/>
       <c r="H113" s="4"/>
       <c r="I113" s="4"/>
@@ -3022,8 +3022,8 @@
       <c r="B114" s="6"/>
       <c r="C114" s="4"/>
       <c r="D114" s="4"/>
-      <c r="E114" s="12"/>
-      <c r="F114" s="12"/>
+      <c r="E114" s="11"/>
+      <c r="F114" s="11"/>
       <c r="G114" s="4"/>
       <c r="H114" s="4"/>
       <c r="I114" s="4"/>
@@ -3033,8 +3033,8 @@
       <c r="B115" s="6"/>
       <c r="C115" s="4"/>
       <c r="D115" s="4"/>
-      <c r="E115" s="12"/>
-      <c r="F115" s="12"/>
+      <c r="E115" s="11"/>
+      <c r="F115" s="11"/>
       <c r="G115" s="4"/>
       <c r="H115" s="4"/>
       <c r="I115" s="4"/>
@@ -3044,8 +3044,8 @@
       <c r="B116" s="6"/>
       <c r="C116" s="4"/>
       <c r="D116" s="4"/>
-      <c r="E116" s="12"/>
-      <c r="F116" s="12"/>
+      <c r="E116" s="11"/>
+      <c r="F116" s="11"/>
       <c r="G116" s="4"/>
       <c r="H116" s="4"/>
       <c r="I116" s="4"/>
@@ -3055,8 +3055,8 @@
       <c r="B117" s="6"/>
       <c r="C117" s="4"/>
       <c r="D117" s="4"/>
-      <c r="E117" s="12"/>
-      <c r="F117" s="12"/>
+      <c r="E117" s="11"/>
+      <c r="F117" s="11"/>
       <c r="G117" s="4"/>
       <c r="H117" s="4"/>
       <c r="I117" s="4"/>
@@ -3066,8 +3066,8 @@
       <c r="B118" s="6"/>
       <c r="C118" s="4"/>
       <c r="D118" s="4"/>
-      <c r="E118" s="12"/>
-      <c r="F118" s="12"/>
+      <c r="E118" s="11"/>
+      <c r="F118" s="11"/>
       <c r="G118" s="4"/>
       <c r="H118" s="4"/>
       <c r="I118" s="4"/>
@@ -3077,8 +3077,8 @@
       <c r="B119" s="6"/>
       <c r="C119" s="4"/>
       <c r="D119" s="4"/>
-      <c r="E119" s="12"/>
-      <c r="F119" s="12"/>
+      <c r="E119" s="11"/>
+      <c r="F119" s="11"/>
       <c r="G119" s="4"/>
       <c r="H119" s="4"/>
       <c r="I119" s="4"/>
@@ -3088,8 +3088,8 @@
       <c r="B120" s="6"/>
       <c r="C120" s="4"/>
       <c r="D120" s="4"/>
-      <c r="E120" s="12"/>
-      <c r="F120" s="12"/>
+      <c r="E120" s="11"/>
+      <c r="F120" s="11"/>
       <c r="G120" s="4"/>
       <c r="H120" s="4"/>
       <c r="I120" s="4"/>
@@ -3099,8 +3099,8 @@
       <c r="B121" s="6"/>
       <c r="C121" s="4"/>
       <c r="D121" s="4"/>
-      <c r="E121" s="12"/>
-      <c r="F121" s="12"/>
+      <c r="E121" s="11"/>
+      <c r="F121" s="11"/>
       <c r="G121" s="4"/>
       <c r="H121" s="4"/>
       <c r="I121" s="4"/>
@@ -3110,8 +3110,8 @@
       <c r="B122" s="6"/>
       <c r="C122" s="4"/>
       <c r="D122" s="4"/>
-      <c r="E122" s="12"/>
-      <c r="F122" s="12"/>
+      <c r="E122" s="11"/>
+      <c r="F122" s="11"/>
       <c r="G122" s="4"/>
       <c r="H122" s="4"/>
       <c r="I122" s="4"/>
@@ -3121,8 +3121,8 @@
       <c r="B123" s="6"/>
       <c r="C123" s="4"/>
       <c r="D123" s="4"/>
-      <c r="E123" s="12"/>
-      <c r="F123" s="12"/>
+      <c r="E123" s="11"/>
+      <c r="F123" s="11"/>
       <c r="G123" s="4"/>
       <c r="H123" s="4"/>
       <c r="I123" s="4"/>
@@ -3132,8 +3132,8 @@
       <c r="B124" s="6"/>
       <c r="C124" s="4"/>
       <c r="D124" s="4"/>
-      <c r="E124" s="12"/>
-      <c r="F124" s="12"/>
+      <c r="E124" s="11"/>
+      <c r="F124" s="11"/>
       <c r="G124" s="4"/>
       <c r="H124" s="4"/>
       <c r="I124" s="4"/>
@@ -3143,8 +3143,8 @@
       <c r="B125" s="6"/>
       <c r="C125" s="4"/>
       <c r="D125" s="4"/>
-      <c r="E125" s="12"/>
-      <c r="F125" s="12"/>
+      <c r="E125" s="11"/>
+      <c r="F125" s="11"/>
       <c r="G125" s="4"/>
       <c r="H125" s="4"/>
       <c r="I125" s="4"/>
@@ -3154,8 +3154,8 @@
       <c r="B126" s="6"/>
       <c r="C126" s="4"/>
       <c r="D126" s="4"/>
-      <c r="E126" s="12"/>
-      <c r="F126" s="12"/>
+      <c r="E126" s="11"/>
+      <c r="F126" s="11"/>
       <c r="G126" s="4"/>
       <c r="H126" s="4"/>
       <c r="I126" s="4"/>
@@ -3165,8 +3165,8 @@
       <c r="B127" s="6"/>
       <c r="C127" s="4"/>
       <c r="D127" s="4"/>
-      <c r="E127" s="12"/>
-      <c r="F127" s="12"/>
+      <c r="E127" s="11"/>
+      <c r="F127" s="11"/>
       <c r="G127" s="4"/>
       <c r="H127" s="4"/>
       <c r="I127" s="4"/>
@@ -3176,8 +3176,8 @@
       <c r="B128" s="6"/>
       <c r="C128" s="4"/>
       <c r="D128" s="4"/>
-      <c r="E128" s="12"/>
-      <c r="F128" s="12"/>
+      <c r="E128" s="11"/>
+      <c r="F128" s="11"/>
       <c r="G128" s="4"/>
       <c r="H128" s="4"/>
       <c r="I128" s="4"/>
@@ -3187,8 +3187,8 @@
       <c r="B129" s="6"/>
       <c r="C129" s="4"/>
       <c r="D129" s="4"/>
-      <c r="E129" s="12"/>
-      <c r="F129" s="12"/>
+      <c r="E129" s="11"/>
+      <c r="F129" s="11"/>
       <c r="G129" s="4"/>
       <c r="H129" s="4"/>
       <c r="I129" s="4"/>
@@ -3198,8 +3198,8 @@
       <c r="B130" s="6"/>
       <c r="C130" s="4"/>
       <c r="D130" s="4"/>
-      <c r="E130" s="12"/>
-      <c r="F130" s="12"/>
+      <c r="E130" s="11"/>
+      <c r="F130" s="11"/>
       <c r="G130" s="4"/>
       <c r="H130" s="4"/>
       <c r="I130" s="4"/>
@@ -3209,8 +3209,8 @@
       <c r="B131" s="6"/>
       <c r="C131" s="4"/>
       <c r="D131" s="4"/>
-      <c r="E131" s="12"/>
-      <c r="F131" s="12"/>
+      <c r="E131" s="11"/>
+      <c r="F131" s="11"/>
       <c r="G131" s="4"/>
       <c r="H131" s="4"/>
       <c r="I131" s="4"/>
@@ -3220,8 +3220,8 @@
       <c r="B132" s="6"/>
       <c r="C132" s="4"/>
       <c r="D132" s="4"/>
-      <c r="E132" s="12"/>
-      <c r="F132" s="12"/>
+      <c r="E132" s="11"/>
+      <c r="F132" s="11"/>
       <c r="G132" s="4"/>
       <c r="H132" s="4"/>
       <c r="I132" s="4"/>
@@ -3231,8 +3231,8 @@
       <c r="B133" s="6"/>
       <c r="C133" s="4"/>
       <c r="D133" s="4"/>
-      <c r="E133" s="12"/>
-      <c r="F133" s="12"/>
+      <c r="E133" s="11"/>
+      <c r="F133" s="11"/>
       <c r="G133" s="4"/>
       <c r="H133" s="4"/>
       <c r="I133" s="4"/>
@@ -3242,8 +3242,8 @@
       <c r="B134" s="6"/>
       <c r="C134" s="4"/>
       <c r="D134" s="4"/>
-      <c r="E134" s="12"/>
-      <c r="F134" s="12"/>
+      <c r="E134" s="11"/>
+      <c r="F134" s="11"/>
       <c r="G134" s="4"/>
       <c r="H134" s="4"/>
       <c r="I134" s="4"/>
@@ -3253,8 +3253,8 @@
       <c r="B135" s="6"/>
       <c r="C135" s="4"/>
       <c r="D135" s="4"/>
-      <c r="E135" s="12"/>
-      <c r="F135" s="12"/>
+      <c r="E135" s="11"/>
+      <c r="F135" s="11"/>
       <c r="G135" s="4"/>
       <c r="H135" s="4"/>
       <c r="I135" s="4"/>
@@ -3264,8 +3264,8 @@
       <c r="B136" s="6"/>
       <c r="C136" s="4"/>
       <c r="D136" s="4"/>
-      <c r="E136" s="12"/>
-      <c r="F136" s="12"/>
+      <c r="E136" s="11"/>
+      <c r="F136" s="11"/>
       <c r="G136" s="4"/>
       <c r="H136" s="4"/>
       <c r="I136" s="4"/>
@@ -3275,8 +3275,8 @@
       <c r="B137" s="6"/>
       <c r="C137" s="4"/>
       <c r="D137" s="4"/>
-      <c r="E137" s="12"/>
-      <c r="F137" s="12"/>
+      <c r="E137" s="11"/>
+      <c r="F137" s="11"/>
       <c r="G137" s="4"/>
       <c r="H137" s="4"/>
       <c r="I137" s="4"/>
@@ -3286,8 +3286,8 @@
       <c r="B138" s="6"/>
       <c r="C138" s="4"/>
       <c r="D138" s="4"/>
-      <c r="E138" s="12"/>
-      <c r="F138" s="12"/>
+      <c r="E138" s="11"/>
+      <c r="F138" s="11"/>
       <c r="G138" s="4"/>
       <c r="H138" s="4"/>
       <c r="I138" s="4"/>
@@ -3297,8 +3297,8 @@
       <c r="B139" s="6"/>
       <c r="C139" s="4"/>
       <c r="D139" s="4"/>
-      <c r="E139" s="12"/>
-      <c r="F139" s="12"/>
+      <c r="E139" s="11"/>
+      <c r="F139" s="11"/>
       <c r="G139" s="4"/>
       <c r="H139" s="4"/>
       <c r="I139" s="4"/>
@@ -3308,8 +3308,8 @@
       <c r="B140" s="6"/>
       <c r="C140" s="4"/>
       <c r="D140" s="4"/>
-      <c r="E140" s="12"/>
-      <c r="F140" s="12"/>
+      <c r="E140" s="11"/>
+      <c r="F140" s="11"/>
       <c r="G140" s="4"/>
       <c r="H140" s="4"/>
       <c r="I140" s="4"/>
@@ -3319,8 +3319,8 @@
       <c r="B141" s="6"/>
       <c r="C141" s="4"/>
       <c r="D141" s="4"/>
-      <c r="E141" s="12"/>
-      <c r="F141" s="12"/>
+      <c r="E141" s="11"/>
+      <c r="F141" s="11"/>
       <c r="G141" s="4"/>
       <c r="H141" s="4"/>
       <c r="I141" s="4"/>
@@ -3330,8 +3330,8 @@
       <c r="B142" s="6"/>
       <c r="C142" s="4"/>
       <c r="D142" s="4"/>
-      <c r="E142" s="12"/>
-      <c r="F142" s="12"/>
+      <c r="E142" s="11"/>
+      <c r="F142" s="11"/>
       <c r="G142" s="4"/>
       <c r="H142" s="4"/>
       <c r="I142" s="4"/>
@@ -3341,8 +3341,8 @@
       <c r="B143" s="6"/>
       <c r="C143" s="4"/>
       <c r="D143" s="4"/>
-      <c r="E143" s="12"/>
-      <c r="F143" s="12"/>
+      <c r="E143" s="11"/>
+      <c r="F143" s="11"/>
       <c r="G143" s="4"/>
       <c r="H143" s="4"/>
       <c r="I143" s="4"/>
@@ -3352,8 +3352,8 @@
       <c r="B144" s="6"/>
       <c r="C144" s="4"/>
       <c r="D144" s="4"/>
-      <c r="E144" s="12"/>
-      <c r="F144" s="12"/>
+      <c r="E144" s="11"/>
+      <c r="F144" s="11"/>
       <c r="G144" s="4"/>
       <c r="H144" s="4"/>
       <c r="I144" s="4"/>
@@ -3363,8 +3363,8 @@
       <c r="B145" s="6"/>
       <c r="C145" s="4"/>
       <c r="D145" s="4"/>
-      <c r="E145" s="12"/>
-      <c r="F145" s="12"/>
+      <c r="E145" s="11"/>
+      <c r="F145" s="11"/>
       <c r="G145" s="4"/>
       <c r="H145" s="4"/>
       <c r="I145" s="4"/>
@@ -3374,8 +3374,8 @@
       <c r="B146" s="6"/>
       <c r="C146" s="4"/>
       <c r="D146" s="4"/>
-      <c r="E146" s="12"/>
-      <c r="F146" s="12"/>
+      <c r="E146" s="11"/>
+      <c r="F146" s="11"/>
       <c r="G146" s="4"/>
       <c r="H146" s="4"/>
       <c r="I146" s="4"/>
@@ -3385,8 +3385,8 @@
       <c r="B147" s="6"/>
       <c r="C147" s="4"/>
       <c r="D147" s="4"/>
-      <c r="E147" s="12"/>
-      <c r="F147" s="12"/>
+      <c r="E147" s="11"/>
+      <c r="F147" s="11"/>
       <c r="G147" s="4"/>
       <c r="H147" s="4"/>
       <c r="I147" s="4"/>
@@ -3396,8 +3396,8 @@
       <c r="B148" s="6"/>
       <c r="C148" s="4"/>
       <c r="D148" s="4"/>
-      <c r="E148" s="12"/>
-      <c r="F148" s="12"/>
+      <c r="E148" s="11"/>
+      <c r="F148" s="11"/>
       <c r="G148" s="4"/>
       <c r="H148" s="4"/>
       <c r="I148" s="4"/>
@@ -3407,8 +3407,8 @@
       <c r="B149" s="6"/>
       <c r="C149" s="4"/>
       <c r="D149" s="4"/>
-      <c r="E149" s="12"/>
-      <c r="F149" s="12"/>
+      <c r="E149" s="11"/>
+      <c r="F149" s="11"/>
       <c r="G149" s="4"/>
       <c r="H149" s="4"/>
       <c r="I149" s="4"/>
@@ -3418,8 +3418,8 @@
       <c r="B150" s="6"/>
       <c r="C150" s="4"/>
       <c r="D150" s="4"/>
-      <c r="E150" s="12"/>
-      <c r="F150" s="12"/>
+      <c r="E150" s="11"/>
+      <c r="F150" s="11"/>
       <c r="G150" s="4"/>
       <c r="H150" s="4"/>
       <c r="I150" s="4"/>
@@ -3429,8 +3429,8 @@
       <c r="B151" s="6"/>
       <c r="C151" s="4"/>
       <c r="D151" s="4"/>
-      <c r="E151" s="12"/>
-      <c r="F151" s="12"/>
+      <c r="E151" s="11"/>
+      <c r="F151" s="11"/>
       <c r="G151" s="4"/>
       <c r="H151" s="4"/>
       <c r="I151" s="4"/>
@@ -3440,8 +3440,8 @@
       <c r="B152" s="6"/>
       <c r="C152" s="4"/>
       <c r="D152" s="4"/>
-      <c r="E152" s="12"/>
-      <c r="F152" s="12"/>
+      <c r="E152" s="11"/>
+      <c r="F152" s="11"/>
       <c r="G152" s="4"/>
       <c r="H152" s="4"/>
       <c r="I152" s="4"/>
@@ -3451,8 +3451,8 @@
       <c r="B153" s="6"/>
       <c r="C153" s="4"/>
       <c r="D153" s="4"/>
-      <c r="E153" s="12"/>
-      <c r="F153" s="12"/>
+      <c r="E153" s="11"/>
+      <c r="F153" s="11"/>
       <c r="G153" s="4"/>
       <c r="H153" s="4"/>
       <c r="I153" s="4"/>
@@ -3462,8 +3462,8 @@
       <c r="B154" s="6"/>
       <c r="C154" s="4"/>
       <c r="D154" s="4"/>
-      <c r="E154" s="12"/>
-      <c r="F154" s="12"/>
+      <c r="E154" s="11"/>
+      <c r="F154" s="11"/>
       <c r="G154" s="4"/>
       <c r="H154" s="4"/>
       <c r="I154" s="4"/>
@@ -3473,8 +3473,8 @@
       <c r="B155" s="6"/>
       <c r="C155" s="4"/>
       <c r="D155" s="4"/>
-      <c r="E155" s="12"/>
-      <c r="F155" s="12"/>
+      <c r="E155" s="11"/>
+      <c r="F155" s="11"/>
       <c r="G155" s="4"/>
       <c r="H155" s="4"/>
       <c r="I155" s="4"/>
@@ -3484,8 +3484,8 @@
       <c r="B156" s="6"/>
       <c r="C156" s="4"/>
       <c r="D156" s="4"/>
-      <c r="E156" s="12"/>
-      <c r="F156" s="12"/>
+      <c r="E156" s="11"/>
+      <c r="F156" s="11"/>
       <c r="G156" s="4"/>
       <c r="H156" s="4"/>
       <c r="I156" s="4"/>
@@ -3495,8 +3495,8 @@
       <c r="B157" s="6"/>
       <c r="C157" s="4"/>
       <c r="D157" s="4"/>
-      <c r="E157" s="12"/>
-      <c r="F157" s="12"/>
+      <c r="E157" s="11"/>
+      <c r="F157" s="11"/>
       <c r="G157" s="4"/>
       <c r="H157" s="4"/>
       <c r="I157" s="4"/>
@@ -3506,8 +3506,8 @@
       <c r="B158" s="6"/>
       <c r="C158" s="4"/>
       <c r="D158" s="4"/>
-      <c r="E158" s="12"/>
-      <c r="F158" s="12"/>
+      <c r="E158" s="11"/>
+      <c r="F158" s="11"/>
       <c r="G158" s="4"/>
       <c r="H158" s="4"/>
       <c r="I158" s="4"/>
@@ -3517,8 +3517,8 @@
       <c r="B159" s="6"/>
       <c r="C159" s="4"/>
       <c r="D159" s="4"/>
-      <c r="E159" s="12"/>
-      <c r="F159" s="12"/>
+      <c r="E159" s="11"/>
+      <c r="F159" s="11"/>
       <c r="G159" s="4"/>
       <c r="H159" s="4"/>
       <c r="I159" s="4"/>
@@ -3528,8 +3528,8 @@
       <c r="B160" s="6"/>
       <c r="C160" s="4"/>
       <c r="D160" s="4"/>
-      <c r="E160" s="12"/>
-      <c r="F160" s="12"/>
+      <c r="E160" s="11"/>
+      <c r="F160" s="11"/>
       <c r="G160" s="4"/>
       <c r="H160" s="4"/>
       <c r="I160" s="4"/>
@@ -3539,8 +3539,8 @@
       <c r="B161" s="6"/>
       <c r="C161" s="4"/>
       <c r="D161" s="4"/>
-      <c r="E161" s="12"/>
-      <c r="F161" s="12"/>
+      <c r="E161" s="11"/>
+      <c r="F161" s="11"/>
       <c r="G161" s="4"/>
       <c r="H161" s="4"/>
       <c r="I161" s="4"/>
@@ -3550,8 +3550,8 @@
       <c r="B162" s="6"/>
       <c r="C162" s="4"/>
       <c r="D162" s="4"/>
-      <c r="E162" s="12"/>
-      <c r="F162" s="12"/>
+      <c r="E162" s="11"/>
+      <c r="F162" s="11"/>
       <c r="G162" s="4"/>
       <c r="H162" s="4"/>
       <c r="I162" s="4"/>
@@ -3561,8 +3561,8 @@
       <c r="B163" s="6"/>
       <c r="C163" s="4"/>
       <c r="D163" s="4"/>
-      <c r="E163" s="12"/>
-      <c r="F163" s="12"/>
+      <c r="E163" s="11"/>
+      <c r="F163" s="11"/>
       <c r="G163" s="4"/>
       <c r="H163" s="4"/>
       <c r="I163" s="4"/>
@@ -3572,7 +3572,7 @@
       <c r="B164" s="6"/>
       <c r="C164" s="4"/>
       <c r="D164" s="4"/>
-      <c r="E164" s="12"/>
+      <c r="E164" s="11"/>
       <c r="F164" s="4"/>
       <c r="G164" s="4"/>
       <c r="H164" s="4"/>
@@ -3583,7 +3583,7 @@
       <c r="B165" s="6"/>
       <c r="C165" s="4"/>
       <c r="D165" s="4"/>
-      <c r="E165" s="12"/>
+      <c r="E165" s="11"/>
       <c r="F165" s="4"/>
       <c r="G165" s="4"/>
       <c r="H165" s="4"/>
@@ -3594,7 +3594,7 @@
       <c r="B166" s="6"/>
       <c r="C166" s="4"/>
       <c r="D166" s="4"/>
-      <c r="E166" s="12"/>
+      <c r="E166" s="11"/>
       <c r="F166" s="4"/>
       <c r="G166" s="4"/>
       <c r="H166" s="4"/>
@@ -3605,7 +3605,7 @@
       <c r="B167" s="6"/>
       <c r="C167" s="4"/>
       <c r="D167" s="4"/>
-      <c r="E167" s="12"/>
+      <c r="E167" s="11"/>
       <c r="F167" s="4"/>
       <c r="G167" s="4"/>
       <c r="H167" s="4"/>
@@ -3616,7 +3616,7 @@
       <c r="B168" s="6"/>
       <c r="C168" s="4"/>
       <c r="D168" s="4"/>
-      <c r="E168" s="12"/>
+      <c r="E168" s="11"/>
       <c r="F168" s="4"/>
       <c r="G168" s="4"/>
       <c r="H168" s="4"/>
@@ -3627,7 +3627,7 @@
       <c r="B169" s="6"/>
       <c r="C169" s="4"/>
       <c r="D169" s="4"/>
-      <c r="E169" s="12"/>
+      <c r="E169" s="11"/>
       <c r="F169" s="4"/>
       <c r="G169" s="4"/>
       <c r="H169" s="4"/>
@@ -3638,7 +3638,7 @@
       <c r="B170" s="6"/>
       <c r="C170" s="4"/>
       <c r="D170" s="4"/>
-      <c r="E170" s="12"/>
+      <c r="E170" s="11"/>
       <c r="F170" s="4"/>
       <c r="G170" s="4"/>
       <c r="H170" s="4"/>
@@ -3649,7 +3649,7 @@
       <c r="B171" s="6"/>
       <c r="C171" s="4"/>
       <c r="D171" s="4"/>
-      <c r="E171" s="12"/>
+      <c r="E171" s="11"/>
       <c r="F171" s="4"/>
       <c r="G171" s="4"/>
       <c r="H171" s="4"/>
@@ -3660,7 +3660,7 @@
       <c r="B172" s="6"/>
       <c r="C172" s="4"/>
       <c r="D172" s="4"/>
-      <c r="E172" s="12"/>
+      <c r="E172" s="11"/>
       <c r="F172" s="4"/>
       <c r="G172" s="4"/>
       <c r="H172" s="4"/>
@@ -3671,7 +3671,7 @@
       <c r="B173" s="6"/>
       <c r="C173" s="4"/>
       <c r="D173" s="4"/>
-      <c r="E173" s="12"/>
+      <c r="E173" s="11"/>
       <c r="F173" s="4"/>
       <c r="G173" s="4"/>
       <c r="H173" s="4"/>
@@ -3682,7 +3682,7 @@
       <c r="B174" s="6"/>
       <c r="C174" s="4"/>
       <c r="D174" s="4"/>
-      <c r="E174" s="12"/>
+      <c r="E174" s="11"/>
       <c r="F174" s="4"/>
       <c r="G174" s="4"/>
       <c r="H174" s="4"/>
@@ -3693,7 +3693,7 @@
       <c r="B175" s="6"/>
       <c r="C175" s="4"/>
       <c r="D175" s="4"/>
-      <c r="E175" s="12"/>
+      <c r="E175" s="11"/>
       <c r="F175" s="4"/>
       <c r="G175" s="4"/>
       <c r="H175" s="4"/>
@@ -3704,7 +3704,7 @@
       <c r="B176" s="6"/>
       <c r="C176" s="4"/>
       <c r="D176" s="4"/>
-      <c r="E176" s="12"/>
+      <c r="E176" s="11"/>
       <c r="F176" s="4"/>
       <c r="G176" s="4"/>
       <c r="H176" s="4"/>
@@ -3715,7 +3715,7 @@
       <c r="B177" s="6"/>
       <c r="C177" s="4"/>
       <c r="D177" s="4"/>
-      <c r="E177" s="12"/>
+      <c r="E177" s="11"/>
       <c r="F177" s="4"/>
       <c r="G177" s="4"/>
       <c r="H177" s="4"/>
@@ -3726,7 +3726,7 @@
       <c r="B178" s="6"/>
       <c r="C178" s="4"/>
       <c r="D178" s="4"/>
-      <c r="E178" s="12"/>
+      <c r="E178" s="11"/>
       <c r="F178" s="4"/>
       <c r="G178" s="4"/>
       <c r="H178" s="4"/>
@@ -3737,7 +3737,7 @@
       <c r="B179" s="6"/>
       <c r="C179" s="4"/>
       <c r="D179" s="4"/>
-      <c r="E179" s="12"/>
+      <c r="E179" s="11"/>
       <c r="F179" s="4"/>
       <c r="G179" s="4"/>
       <c r="H179" s="4"/>
@@ -3748,7 +3748,7 @@
       <c r="B180" s="6"/>
       <c r="C180" s="4"/>
       <c r="D180" s="4"/>
-      <c r="E180" s="12"/>
+      <c r="E180" s="11"/>
       <c r="F180" s="4"/>
       <c r="G180" s="4"/>
       <c r="H180" s="4"/>
@@ -3759,7 +3759,7 @@
       <c r="B181" s="6"/>
       <c r="C181" s="4"/>
       <c r="D181" s="4"/>
-      <c r="E181" s="12"/>
+      <c r="E181" s="11"/>
       <c r="F181" s="4"/>
       <c r="G181" s="4"/>
       <c r="H181" s="4"/>
@@ -3770,7 +3770,7 @@
       <c r="B182" s="6"/>
       <c r="C182" s="4"/>
       <c r="D182" s="4"/>
-      <c r="E182" s="12"/>
+      <c r="E182" s="11"/>
       <c r="F182" s="4"/>
       <c r="G182" s="4"/>
       <c r="H182" s="4"/>
@@ -3781,7 +3781,7 @@
       <c r="B183" s="6"/>
       <c r="C183" s="4"/>
       <c r="D183" s="4"/>
-      <c r="E183" s="12"/>
+      <c r="E183" s="11"/>
       <c r="F183" s="4"/>
       <c r="G183" s="4"/>
       <c r="H183" s="4"/>
@@ -3792,7 +3792,7 @@
       <c r="B184" s="6"/>
       <c r="C184" s="4"/>
       <c r="D184" s="4"/>
-      <c r="E184" s="12"/>
+      <c r="E184" s="11"/>
       <c r="F184" s="4"/>
       <c r="G184" s="4"/>
       <c r="H184" s="4"/>
@@ -3803,7 +3803,7 @@
       <c r="B185" s="6"/>
       <c r="C185" s="4"/>
       <c r="D185" s="4"/>
-      <c r="E185" s="12"/>
+      <c r="E185" s="11"/>
       <c r="F185" s="4"/>
       <c r="G185" s="4"/>
       <c r="H185" s="4"/>
@@ -3814,7 +3814,7 @@
       <c r="B186" s="6"/>
       <c r="C186" s="4"/>
       <c r="D186" s="4"/>
-      <c r="E186" s="12"/>
+      <c r="E186" s="11"/>
       <c r="F186" s="4"/>
       <c r="G186" s="4"/>
       <c r="H186" s="4"/>
@@ -3825,7 +3825,7 @@
       <c r="B187" s="6"/>
       <c r="C187" s="4"/>
       <c r="D187" s="4"/>
-      <c r="E187" s="12"/>
+      <c r="E187" s="11"/>
       <c r="F187" s="4"/>
       <c r="G187" s="4"/>
       <c r="H187" s="4"/>
@@ -3836,7 +3836,7 @@
       <c r="B188" s="6"/>
       <c r="C188" s="4"/>
       <c r="D188" s="4"/>
-      <c r="E188" s="12"/>
+      <c r="E188" s="11"/>
       <c r="F188" s="4"/>
       <c r="G188" s="4"/>
       <c r="H188" s="4"/>
@@ -3847,7 +3847,7 @@
       <c r="B189" s="6"/>
       <c r="C189" s="4"/>
       <c r="D189" s="4"/>
-      <c r="E189" s="12"/>
+      <c r="E189" s="11"/>
       <c r="F189" s="4"/>
       <c r="G189" s="4"/>
       <c r="H189" s="4"/>
@@ -3858,7 +3858,7 @@
       <c r="B190" s="6"/>
       <c r="C190" s="4"/>
       <c r="D190" s="4"/>
-      <c r="E190" s="12"/>
+      <c r="E190" s="11"/>
       <c r="F190" s="4"/>
       <c r="G190" s="4"/>
       <c r="H190" s="4"/>
@@ -3869,7 +3869,7 @@
       <c r="B191" s="6"/>
       <c r="C191" s="4"/>
       <c r="D191" s="4"/>
-      <c r="E191" s="12"/>
+      <c r="E191" s="11"/>
       <c r="F191" s="4"/>
       <c r="G191" s="4"/>
       <c r="H191" s="4"/>
@@ -3880,7 +3880,7 @@
       <c r="B192" s="6"/>
       <c r="C192" s="4"/>
       <c r="D192" s="4"/>
-      <c r="E192" s="12"/>
+      <c r="E192" s="11"/>
       <c r="F192" s="4"/>
       <c r="G192" s="4"/>
       <c r="H192" s="4"/>
@@ -3891,7 +3891,7 @@
       <c r="B193" s="6"/>
       <c r="C193" s="4"/>
       <c r="D193" s="4"/>
-      <c r="E193" s="12"/>
+      <c r="E193" s="11"/>
       <c r="F193" s="4"/>
       <c r="G193" s="4"/>
       <c r="H193" s="4"/>
@@ -3902,7 +3902,7 @@
       <c r="B194" s="6"/>
       <c r="C194" s="4"/>
       <c r="D194" s="4"/>
-      <c r="E194" s="12"/>
+      <c r="E194" s="11"/>
       <c r="F194" s="4"/>
       <c r="G194" s="4"/>
       <c r="H194" s="4"/>
@@ -3913,7 +3913,7 @@
       <c r="B195" s="6"/>
       <c r="C195" s="4"/>
       <c r="D195" s="4"/>
-      <c r="E195" s="12"/>
+      <c r="E195" s="11"/>
       <c r="F195" s="4"/>
       <c r="G195" s="4"/>
       <c r="H195" s="4"/>
@@ -3924,7 +3924,7 @@
       <c r="B196" s="6"/>
       <c r="C196" s="4"/>
       <c r="D196" s="4"/>
-      <c r="E196" s="12"/>
+      <c r="E196" s="11"/>
       <c r="F196" s="4"/>
       <c r="G196" s="4"/>
       <c r="H196" s="4"/>
@@ -3935,7 +3935,7 @@
       <c r="B197" s="6"/>
       <c r="C197" s="4"/>
       <c r="D197" s="4"/>
-      <c r="E197" s="12"/>
+      <c r="E197" s="11"/>
       <c r="F197" s="4"/>
       <c r="G197" s="4"/>
       <c r="H197" s="4"/>
@@ -3946,7 +3946,7 @@
       <c r="B198" s="6"/>
       <c r="C198" s="4"/>
       <c r="D198" s="4"/>
-      <c r="E198" s="12"/>
+      <c r="E198" s="11"/>
       <c r="F198" s="4"/>
       <c r="G198" s="4"/>
       <c r="H198" s="4"/>
@@ -3957,7 +3957,7 @@
       <c r="B199" s="6"/>
       <c r="C199" s="4"/>
       <c r="D199" s="4"/>
-      <c r="E199" s="12"/>
+      <c r="E199" s="11"/>
       <c r="F199" s="4"/>
       <c r="G199" s="4"/>
       <c r="H199" s="4"/>
@@ -3968,7 +3968,7 @@
       <c r="B200" s="6"/>
       <c r="C200" s="4"/>
       <c r="D200" s="4"/>
-      <c r="E200" s="12"/>
+      <c r="E200" s="11"/>
       <c r="F200" s="4"/>
       <c r="G200" s="4"/>
       <c r="H200" s="4"/>
@@ -3979,7 +3979,7 @@
       <c r="B201" s="6"/>
       <c r="C201" s="4"/>
       <c r="D201" s="4"/>
-      <c r="E201" s="12"/>
+      <c r="E201" s="11"/>
       <c r="F201" s="4"/>
       <c r="G201" s="4"/>
       <c r="H201" s="4"/>
@@ -3990,7 +3990,7 @@
       <c r="B202" s="6"/>
       <c r="C202" s="4"/>
       <c r="D202" s="4"/>
-      <c r="E202" s="12"/>
+      <c r="E202" s="11"/>
       <c r="F202" s="4"/>
       <c r="G202" s="4"/>
       <c r="H202" s="4"/>
@@ -4001,7 +4001,7 @@
       <c r="B203" s="6"/>
       <c r="C203" s="4"/>
       <c r="D203" s="4"/>
-      <c r="E203" s="12"/>
+      <c r="E203" s="11"/>
       <c r="F203" s="4"/>
       <c r="G203" s="4"/>
       <c r="H203" s="4"/>
@@ -4012,7 +4012,7 @@
       <c r="B204" s="6"/>
       <c r="C204" s="4"/>
       <c r="D204" s="4"/>
-      <c r="E204" s="12"/>
+      <c r="E204" s="11"/>
       <c r="F204" s="4"/>
       <c r="G204" s="4"/>
       <c r="H204" s="4"/>
@@ -4023,7 +4023,7 @@
       <c r="B205" s="6"/>
       <c r="C205" s="4"/>
       <c r="D205" s="4"/>
-      <c r="E205" s="12"/>
+      <c r="E205" s="11"/>
       <c r="F205" s="4"/>
       <c r="G205" s="4"/>
       <c r="H205" s="4"/>
@@ -4034,7 +4034,7 @@
       <c r="B206" s="6"/>
       <c r="C206" s="4"/>
       <c r="D206" s="4"/>
-      <c r="E206" s="12"/>
+      <c r="E206" s="11"/>
       <c r="F206" s="4"/>
       <c r="G206" s="4"/>
       <c r="H206" s="4"/>
@@ -4045,7 +4045,7 @@
       <c r="B207" s="6"/>
       <c r="C207" s="4"/>
       <c r="D207" s="4"/>
-      <c r="E207" s="12"/>
+      <c r="E207" s="11"/>
       <c r="F207" s="4"/>
       <c r="G207" s="4"/>
       <c r="H207" s="4"/>
@@ -4056,7 +4056,7 @@
       <c r="B208" s="6"/>
       <c r="C208" s="4"/>
       <c r="D208" s="4"/>
-      <c r="E208" s="12"/>
+      <c r="E208" s="11"/>
       <c r="F208" s="4"/>
       <c r="G208" s="4"/>
       <c r="H208" s="4"/>
@@ -4067,7 +4067,7 @@
       <c r="B209" s="6"/>
       <c r="C209" s="4"/>
       <c r="D209" s="4"/>
-      <c r="E209" s="12"/>
+      <c r="E209" s="11"/>
       <c r="F209" s="4"/>
       <c r="G209" s="4"/>
       <c r="H209" s="4"/>
@@ -4078,7 +4078,7 @@
       <c r="B210" s="6"/>
       <c r="C210" s="4"/>
       <c r="D210" s="4"/>
-      <c r="E210" s="12"/>
+      <c r="E210" s="11"/>
       <c r="F210" s="4"/>
       <c r="G210" s="4"/>
       <c r="H210" s="4"/>
@@ -4089,7 +4089,7 @@
       <c r="B211" s="6"/>
       <c r="C211" s="4"/>
       <c r="D211" s="4"/>
-      <c r="E211" s="12"/>
+      <c r="E211" s="11"/>
       <c r="F211" s="4"/>
       <c r="G211" s="4"/>
       <c r="H211" s="4"/>
@@ -4100,7 +4100,7 @@
       <c r="B212" s="6"/>
       <c r="C212" s="4"/>
       <c r="D212" s="4"/>
-      <c r="E212" s="12"/>
+      <c r="E212" s="11"/>
       <c r="F212" s="4"/>
       <c r="G212" s="4"/>
       <c r="H212" s="4"/>
@@ -4111,7 +4111,7 @@
       <c r="B213" s="6"/>
       <c r="C213" s="4"/>
       <c r="D213" s="4"/>
-      <c r="E213" s="12"/>
+      <c r="E213" s="11"/>
       <c r="F213" s="4"/>
       <c r="G213" s="4"/>
       <c r="H213" s="4"/>
@@ -4122,7 +4122,7 @@
       <c r="B214" s="6"/>
       <c r="C214" s="4"/>
       <c r="D214" s="4"/>
-      <c r="E214" s="12"/>
+      <c r="E214" s="11"/>
       <c r="F214" s="4"/>
       <c r="G214" s="4"/>
       <c r="H214" s="4"/>

</xml_diff>